<commit_message>
feat: upstream origin merge (#16)
</commit_message>
<xml_diff>
--- a/xlsx/user_test.xlsx
+++ b/xlsx/user_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yixiang Zhao\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\go\casdoor\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC0BA84-A6D3-4823-927B-33DCCFC24105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B37C8BB-2433-4A3B-AC02-99920262261C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="88">
   <si>
     <t>built-in</t>
   </si>
@@ -266,9 +266,6 @@
   </si>
   <si>
     <t>is_admin</t>
-  </si>
-  <si>
-    <t>is_global_admin</t>
   </si>
   <si>
     <t>is_forbidden</t>
@@ -650,15 +647,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN6"/>
+  <dimension ref="A1:AM6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:39">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -776,11 +773,8 @@
       <c r="AM1" t="s">
         <v>86</v>
       </c>
-      <c r="AN1" t="s">
-        <v>87</v>
-      </c>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:39">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -844,17 +838,14 @@
       <c r="AI2">
         <v>0</v>
       </c>
-      <c r="AJ2">
-        <v>0</v>
+      <c r="AJ2" t="s">
+        <v>12</v>
       </c>
       <c r="AK2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:39">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -918,17 +909,14 @@
       <c r="AI3">
         <v>0</v>
       </c>
-      <c r="AJ3">
-        <v>0</v>
+      <c r="AJ3" t="s">
+        <v>12</v>
       </c>
       <c r="AK3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:39">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -992,17 +980,14 @@
       <c r="AI4">
         <v>0</v>
       </c>
-      <c r="AJ4">
-        <v>0</v>
+      <c r="AJ4" t="s">
+        <v>12</v>
       </c>
       <c r="AK4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:39">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1066,17 +1051,14 @@
       <c r="AI5">
         <v>0</v>
       </c>
-      <c r="AJ5">
-        <v>0</v>
+      <c r="AJ5" t="s">
+        <v>12</v>
       </c>
       <c r="AK5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:39">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1140,14 +1122,11 @@
       <c r="AI6">
         <v>0</v>
       </c>
-      <c r="AJ6">
-        <v>0</v>
+      <c r="AJ6" t="s">
+        <v>12</v>
       </c>
       <c r="AK6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>